<commit_message>
Add eligible categories to weigh-in form
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/weighin/WeighInForm-A4.xlsx
+++ b/owlcms/src/main/resources/templates/weighin/WeighInForm-A4.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Starting Weights" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Starting Weights'!$A$14:$K$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Criteria" vbProcedure="false">'Starting Weights'!$A$1:$CN$86</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Starting Weights'!$A$14:$L$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Criteria" vbProcedure="false">'Starting Weights'!$A$1:$CO$86</definedName>
     <definedName function="false" hidden="false" name="AFF." vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="Affiliation" vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="Barre" vbProcedure="false">#REF!</definedName>
@@ -43,7 +43,7 @@
     <definedName function="false" hidden="false" name="PeséeGroupFilter" vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="progr." vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="PRÉNOM" vbProcedure="false">'starting weights'!#ref!</definedName>
-    <definedName function="false" hidden="false" name="requestedCJ" vbProcedure="false">'Starting Weights'!$Q:$Q</definedName>
+    <definedName function="false" hidden="false" name="requestedCJ" vbProcedure="false">'Starting Weights'!$R:$R</definedName>
     <definedName function="false" hidden="false" name="StartGroupFilter" vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="TAS" vbProcedure="false">'starting weights'!#ref!</definedName>
     <definedName function="false" hidden="false" name="tirage" vbProcedure="false">'starting weights'!#ref!</definedName>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">${t.get("Competition.competitionName")} :</t>
   </si>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">${competition.localizedCompetitionDate}</t>
   </si>
   <si>
-    <t xml:space="preserve">${t.get("WeighinSummary")}</t>
+    <t xml:space="preserve">${t.get("WeighinForm")}</t>
   </si>
   <si>
     <t xml:space="preserve">${t.get("Group")} ${session.name}</t>
@@ -115,6 +115,9 @@
     <t xml:space="preserve">${t.get("Results.Birth")}</t>
   </si>
   <si>
+    <t xml:space="preserve">${t.get("Results.Category")}</t>
+  </si>
+  <si>
     <t xml:space="preserve">${t.get("Results.Entry_abbrev")}</t>
   </si>
   <si>
@@ -146,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">${l.formattedBirth}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${l.eligibleCategoriesAsString}</t>
   </si>
   <si>
     <t xml:space="preserve">${l.entryTotal}</t>
@@ -464,8 +470,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,11 +483,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,19 +491,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -505,35 +507,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,11 +543,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,11 +555,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,15 +567,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -581,23 +583,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,19 +607,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,11 +643,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -933,604 +935,602 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:S112"/>
+  <dimension ref="A1:T112"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="3" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="5" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="14.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="3" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="2" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="2"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="N1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="M2" s="2"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="N2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="16"/>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="M3" s="2"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="N3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="M4" s="2"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="A4" s="16"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="N4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
-      <c r="B5" s="23" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="20"/>
-      <c r="M5" s="2"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="19"/>
+      <c r="N5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="G6" s="2"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="2"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="H6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="2"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" s="38" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
+    <row r="12" s="36" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="37" t="s">
+      <c r="I12" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="J12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="35"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" s="46" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="H13" s="18"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" s="45" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="C14" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="D14" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="E14" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="F14" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
+      <c r="G14" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="R15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="1"/>
-      <c r="S16" s="47"/>
+      <c r="D16" s="2"/>
+      <c r="T16" s="46"/>
     </row>
     <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="S17" s="47"/>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="T17" s="46"/>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="S18" s="47"/>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="T18" s="46"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="1"/>
-      <c r="S19" s="47"/>
+      <c r="D19" s="2"/>
+      <c r="T19" s="46"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="1"/>
-      <c r="S20" s="47"/>
+      <c r="D20" s="2"/>
+      <c r="T20" s="46"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="1"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="1"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="1"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="1"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="1"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="1"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="1"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="1"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="1"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="1"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="1"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="1"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="1"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="1"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="1"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="1"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="1"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="1"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="1"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="1"/>
+      <c r="D40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="1"/>
+      <c r="D41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="1"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="1"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="1"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="1"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="1"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="1"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="1"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="1"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="1"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="1"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="1"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="1"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="1"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="1"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="1"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="1"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="1"/>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="1"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="1"/>
+      <c r="D60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="1"/>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="1"/>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="1"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="1"/>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="1"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="1"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="1"/>
+      <c r="D67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="1"/>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="1"/>
+      <c r="D69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="1"/>
+      <c r="D70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D71" s="1"/>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="1"/>
+      <c r="D72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="1"/>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="1"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D75" s="1"/>
+      <c r="D75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="1"/>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D77" s="1"/>
+      <c r="D77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="1"/>
+      <c r="D78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="1"/>
+      <c r="D79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="1"/>
+      <c r="D80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="1"/>
+      <c r="D81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="1"/>
+      <c r="D82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="1"/>
+      <c r="D83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D84" s="1"/>
+      <c r="D84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="1"/>
+      <c r="D85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="1"/>
+      <c r="D86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="1"/>
+      <c r="D87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="1"/>
+      <c r="D88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="1"/>
+      <c r="D89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D90" s="1"/>
+      <c r="D90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="1"/>
+      <c r="D91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="1"/>
+      <c r="D92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D93" s="1"/>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="1"/>
+      <c r="D94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D95" s="1"/>
+      <c r="D95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D96" s="1"/>
+      <c r="D96" s="2"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D97" s="1"/>
+      <c r="D97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="1"/>
+      <c r="D98" s="2"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="1"/>
+      <c r="D99" s="2"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="1"/>
+      <c r="D100" s="2"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D101" s="1"/>
+      <c r="D101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="1"/>
+      <c r="D102" s="2"/>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="1"/>
+      <c r="D103" s="2"/>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="1"/>
+      <c r="D104" s="2"/>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="1"/>
+      <c r="D105" s="2"/>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="1"/>
+      <c r="D106" s="2"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="1"/>
+      <c r="D107" s="2"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="1"/>
+      <c r="D108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="1"/>
+      <c r="D109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="1"/>
+      <c r="D110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="1"/>
+      <c r="D111" s="2"/>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="1"/>
+      <c r="D112" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D1:L1"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D14 F15" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D14 F15:G15" type="decimal">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6" type="none">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>